<commit_message>
tweaking GAMS commands test files and case
</commit_message>
<xml_diff>
--- a/suppxls/Scen_Refinery.xlsx
+++ b/suppxls/Scen_Refinery.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VEDA\VEDA_Models\Demo_Adv_Veda\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01FE84DF-6B3B-4FBB-BEB4-037E0F9FAD86}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D987ABA0-DA4B-4F81-82DE-F49DD8E040A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7500" yWindow="1335" windowWidth="18135" windowHeight="11025" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1470" yWindow="1470" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BY Data" sheetId="15" r:id="rId1"/>

</xml_diff>

<commit_message>
testing reimport in VO
</commit_message>
<xml_diff>
--- a/suppxls/Scen_Refinery.xlsx
+++ b/suppxls/Scen_Refinery.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\Veda\Veda_models\Demo_Adv_Veda\suppxls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBABDAF5-18EA-406A-8C10-A08556A5277F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{191514CF-D975-4B8D-8829-A7EEEF22D8A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3900" yWindow="3900" windowWidth="21600" windowHeight="12735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>

</xml_diff>